<commit_message>
fix: resolve Vite proxy failing inside Docker network
Proxy targeted localhost:3001 which doesn't exist inside the client
container. Now uses VITE_API_URL env var (set to http://server:3001 in
Docker Compose) with localhost fallback for local dev.
</commit_message>
<xml_diff>
--- a/Div filer/Test Herjedal.xlsx
+++ b/Div filer/Test Herjedal.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrofasting/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrofasting/CODE/ECIT-acquisition/Div filer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43254CEE-5E22-AE4D-95AF-3C7BD7D3EFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB3E969-293D-AA48-9C3D-2AE0E7CBC156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="16000" windowHeight="18980" xr2:uid="{CD6F9456-AB92-5448-9CE2-F0C930A13991}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="27660" windowHeight="18980" xr2:uid="{CD6F9456-AB92-5448-9CE2-F0C930A13991}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Argon (Sellside case)</t>
   </si>
@@ -44,25 +45,7 @@
     <t>Revenue</t>
   </si>
   <si>
-    <t>1 105,0</t>
-  </si>
-  <si>
-    <t>1 284,0</t>
-  </si>
-  <si>
-    <t>1 407,0</t>
-  </si>
-  <si>
-    <t>1 603,0</t>
-  </si>
-  <si>
     <t>% vekst</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Total omsetning</t>
   </si>
   <si>
     <t>EBITDA</t>
@@ -93,6 +76,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0\ %"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -161,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -170,6 +156,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6FB135-D2ED-6547-B998-4E0EF4CCB5C2}">
-  <dimension ref="A3:I15"/>
+  <dimension ref="A3:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +504,7 @@
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -552,7 +539,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
         <v>43</v>
@@ -577,7 +564,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3">
         <v>32</v>
@@ -602,7 +589,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>492</v>
@@ -627,7 +614,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4">
         <f>SUM(B6:B8)</f>
@@ -658,28 +645,26 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="8">
         <f>(C9-B9)/B9</f>
         <v>8.2892416225749554E-2</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="8">
         <f>(D9-C9)/C9</f>
         <v>8.3061889250814328E-2</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="8">
         <f t="shared" ref="E10:G10" si="1">(E9-D9)/D9</f>
         <v>0.10977443609022557</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="8">
         <f t="shared" si="1"/>
         <v>0.11517615176151762</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="8">
         <f t="shared" si="1"/>
         <v>0.12029161603888214</v>
       </c>
@@ -687,115 +672,65 @@
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4">
-        <v>754</v>
-      </c>
-      <c r="C11" s="4">
-        <v>873</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="4" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>71</v>
+      </c>
+      <c r="C12" s="3">
+        <v>74</v>
+      </c>
+      <c r="D12" s="3">
+        <v>77</v>
+      </c>
+      <c r="E12" s="3">
+        <v>95</v>
+      </c>
+      <c r="F12" s="3">
+        <v>123</v>
+      </c>
+      <c r="G12" s="3">
+        <v>157</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0.158</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="F12" s="6">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3">
-        <v>71</v>
-      </c>
-      <c r="C14" s="3">
-        <v>74</v>
-      </c>
-      <c r="D14" s="3">
-        <v>77</v>
-      </c>
-      <c r="E14" s="3">
-        <v>95</v>
-      </c>
-      <c r="F14" s="3">
-        <v>123</v>
-      </c>
-      <c r="G14" s="3">
-        <v>157</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="6">
-        <f>B14/B9</f>
+      <c r="B13" s="8">
+        <f>B12/B9</f>
         <v>0.12522045855379188</v>
       </c>
-      <c r="C15" s="6">
-        <f t="shared" ref="C15:G15" si="2">C14/C9</f>
+      <c r="C13" s="8">
+        <f>C12/C9</f>
         <v>0.12052117263843648</v>
       </c>
-      <c r="D15" s="6">
-        <f t="shared" si="2"/>
+      <c r="D13" s="8">
+        <f>D12/D9</f>
         <v>0.11578947368421053</v>
       </c>
-      <c r="E15" s="6">
-        <f t="shared" si="2"/>
+      <c r="E13" s="8">
+        <f>E12/E9</f>
         <v>0.12872628726287264</v>
       </c>
-      <c r="F15" s="6">
-        <f t="shared" si="2"/>
+      <c r="F13" s="8">
+        <f>F12/F9</f>
         <v>0.14945321992709598</v>
       </c>
-      <c r="G15" s="6">
-        <f t="shared" si="2"/>
+      <c r="G13" s="8">
+        <f>G12/G9</f>
         <v>0.17028199566160521</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>